<commit_message>
Update FM26 Players.xlsx with revised player data
</commit_message>
<xml_diff>
--- a/FM26 Players.xlsx
+++ b/FM26 Players.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="25416" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Paste" sheetId="1" state="visible" r:id="rId1"/>
@@ -9497,10 +9497,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CI79"/>
+  <dimension ref="A1:CN79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BZ2" sqref="BZ2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="CJ2" sqref="CJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -9948,6 +9948,31 @@
           <t>Club</t>
         </is>
       </c>
+      <c r="CJ1" t="inlineStr">
+        <is>
+          <t>Contract Type</t>
+        </is>
+      </c>
+      <c r="CK1" t="inlineStr">
+        <is>
+          <t>Wages</t>
+        </is>
+      </c>
+      <c r="CL1" t="inlineStr">
+        <is>
+          <t>Appearance Bonus</t>
+        </is>
+      </c>
+      <c r="CM1" t="inlineStr">
+        <is>
+          <t>Loyalty Bonus</t>
+        </is>
+      </c>
+      <c r="CN1" t="inlineStr">
+        <is>
+          <t>Months Left (Contract)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -9987,7 +10012,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>9524</v>
+        <v>7100</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -10000,7 +10025,7 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="O2" t="n">
         <v>10000</v>
@@ -10221,6 +10246,25 @@
         <v>1</v>
       </c>
       <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>$146</t>
+        </is>
+      </c>
+      <c r="CL2" t="n">
+        <v>20</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>12</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -10260,7 +10304,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>9858</v>
+        <v>9200</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -10273,7 +10317,7 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>-78</v>
+        <v>-28</v>
       </c>
       <c r="O3" t="n">
         <v>10000</v>
@@ -10494,6 +10538,25 @@
         <v>1</v>
       </c>
       <c r="CI3" t="inlineStr"/>
+      <c r="CJ3" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>$724</t>
+        </is>
+      </c>
+      <c r="CL3" t="n">
+        <v>32</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>12</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -10767,6 +10830,23 @@
         <v>1</v>
       </c>
       <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL4" t="n">
+        <v>671</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -10806,7 +10886,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>9356</v>
+        <v>6700</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -10819,7 +10899,7 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>108</v>
+        <v>189</v>
       </c>
       <c r="O5" t="n">
         <v>10000</v>
@@ -11040,6 +11120,25 @@
         <v>1</v>
       </c>
       <c r="CI5" t="inlineStr"/>
+      <c r="CJ5" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK5" t="inlineStr">
+        <is>
+          <t>$374</t>
+        </is>
+      </c>
+      <c r="CL5" t="n">
+        <v>23</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>18</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -11079,7 +11178,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>9954</v>
+        <v>7500</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -11092,10 +11191,10 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="O6" t="n">
-        <v>9898</v>
+        <v>10000</v>
       </c>
       <c r="P6" t="n">
         <v>9</v>
@@ -11313,6 +11412,25 @@
         <v>4</v>
       </c>
       <c r="CI6" t="inlineStr"/>
+      <c r="CJ6" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK6" t="inlineStr">
+        <is>
+          <t>$397</t>
+        </is>
+      </c>
+      <c r="CL6" t="n">
+        <v>19</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>12</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -11586,6 +11704,23 @@
         <v>1</v>
       </c>
       <c r="CI7" t="inlineStr"/>
+      <c r="CJ7" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK7" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL7" t="n">
+        <v>251</v>
+      </c>
+      <c r="CM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -11859,6 +11994,23 @@
         <v>1</v>
       </c>
       <c r="CI8" t="inlineStr"/>
+      <c r="CJ8" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK8" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL8" t="n">
+        <v>381</v>
+      </c>
+      <c r="CM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN8" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -12132,6 +12284,25 @@
         <v>20</v>
       </c>
       <c r="CI9" t="inlineStr"/>
+      <c r="CJ9" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK9" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN9" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -12171,7 +12342,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>9418</v>
+        <v>6600</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -12184,7 +12355,7 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>-33</v>
+        <v>57</v>
       </c>
       <c r="O10" t="n">
         <v>10000</v>
@@ -12405,6 +12576,25 @@
         <v>1</v>
       </c>
       <c r="CI10" t="inlineStr"/>
+      <c r="CJ10" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK10" t="inlineStr">
+        <is>
+          <t>$1,127</t>
+        </is>
+      </c>
+      <c r="CL10" t="n">
+        <v>51</v>
+      </c>
+      <c r="CM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN10" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -12448,7 +12638,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -12678,6 +12868,25 @@
         <v>1</v>
       </c>
       <c r="CI11" t="inlineStr"/>
+      <c r="CJ11" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK11" t="inlineStr">
+        <is>
+          <t>$1,712</t>
+        </is>
+      </c>
+      <c r="CL11" t="n">
+        <v>86</v>
+      </c>
+      <c r="CM11" t="n">
+        <v>35</v>
+      </c>
+      <c r="CN11" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -12951,6 +13160,23 @@
         <v>1</v>
       </c>
       <c r="CI12" t="inlineStr"/>
+      <c r="CJ12" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK12" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL12" t="n">
+        <v>59</v>
+      </c>
+      <c r="CM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN12" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -12990,7 +13216,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>9510</v>
+        <v>7400</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -13003,7 +13229,7 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="O13" t="n">
         <v>10000</v>
@@ -13224,6 +13450,25 @@
         <v>1</v>
       </c>
       <c r="CI13" t="inlineStr"/>
+      <c r="CJ13" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>$1,081</t>
+        </is>
+      </c>
+      <c r="CL13" t="n">
+        <v>51</v>
+      </c>
+      <c r="CM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN13" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -13497,6 +13742,23 @@
         <v>1</v>
       </c>
       <c r="CI14" t="inlineStr"/>
+      <c r="CJ14" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK14" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL14" t="n">
+        <v>269</v>
+      </c>
+      <c r="CM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN14" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -13770,6 +14032,23 @@
         <v>1</v>
       </c>
       <c r="CI15" t="inlineStr"/>
+      <c r="CJ15" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK15" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL15" t="n">
+        <v>267</v>
+      </c>
+      <c r="CM15" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN15" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -14043,6 +14322,23 @@
         <v>20</v>
       </c>
       <c r="CI16" t="inlineStr"/>
+      <c r="CJ16" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK16" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL16" t="n">
+        <v>273</v>
+      </c>
+      <c r="CM16" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN16" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -14316,6 +14612,23 @@
         <v>20</v>
       </c>
       <c r="CI17" t="inlineStr"/>
+      <c r="CJ17" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK17" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL17" t="n">
+        <v>182</v>
+      </c>
+      <c r="CM17" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN17" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -14368,10 +14681,10 @@
         </is>
       </c>
       <c r="N18" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O18" t="n">
-        <v>9718</v>
+        <v>9700</v>
       </c>
       <c r="P18" t="n">
         <v>8</v>
@@ -14589,6 +14902,25 @@
         <v>20</v>
       </c>
       <c r="CI18" t="inlineStr"/>
+      <c r="CJ18" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK18" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL18" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM18" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -14628,7 +14960,7 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>9392</v>
+        <v>6800</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -14641,7 +14973,7 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="O19" t="n">
         <v>10000</v>
@@ -14862,6 +15194,25 @@
         <v>16</v>
       </c>
       <c r="CI19" t="inlineStr"/>
+      <c r="CJ19" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK19" t="inlineStr">
+        <is>
+          <t>$444</t>
+        </is>
+      </c>
+      <c r="CL19" t="n">
+        <v>20</v>
+      </c>
+      <c r="CM19" t="n">
+        <v>6</v>
+      </c>
+      <c r="CN19" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -14901,7 +15252,7 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>9856</v>
+        <v>9800</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -14914,7 +15265,7 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>-112</v>
+        <v>-106</v>
       </c>
       <c r="O20" t="n">
         <v>9700</v>
@@ -15138,6 +15489,25 @@
         <is>
           <t>Brixham</t>
         </is>
+      </c>
+      <c r="CJ20" t="inlineStr">
+        <is>
+          <t>FullTime</t>
+        </is>
+      </c>
+      <c r="CK20" t="inlineStr">
+        <is>
+          <t>$2,775</t>
+        </is>
+      </c>
+      <c r="CL20" t="n">
+        <v>384</v>
+      </c>
+      <c r="CM20" t="n">
+        <v>175</v>
+      </c>
+      <c r="CN20" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -15178,7 +15548,7 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>9472</v>
+        <v>6700</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -15191,7 +15561,7 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="O21" t="n">
         <v>10000</v>
@@ -15412,6 +15782,25 @@
         <v>1</v>
       </c>
       <c r="CI21" t="inlineStr"/>
+      <c r="CJ21" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK21" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL21" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM21" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN21" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -15451,7 +15840,7 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>9631</v>
+        <v>7200</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -15464,7 +15853,7 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>-20</v>
+        <v>60</v>
       </c>
       <c r="O22" t="n">
         <v>10000</v>
@@ -15685,6 +16074,25 @@
         <v>20</v>
       </c>
       <c r="CI22" t="inlineStr"/>
+      <c r="CJ22" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK22" t="inlineStr">
+        <is>
+          <t>$1,063</t>
+        </is>
+      </c>
+      <c r="CL22" t="n">
+        <v>53</v>
+      </c>
+      <c r="CM22" t="n">
+        <v>23</v>
+      </c>
+      <c r="CN22" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -15724,7 +16132,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>9500</v>
+        <v>7700</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -15737,10 +16145,10 @@
         </is>
       </c>
       <c r="N23" t="n">
-        <v>-32</v>
+        <v>36</v>
       </c>
       <c r="O23" t="n">
-        <v>9200</v>
+        <v>9400</v>
       </c>
       <c r="P23" t="n">
         <v>15</v>
@@ -15958,6 +16366,25 @@
         <v>20</v>
       </c>
       <c r="CI23" t="inlineStr"/>
+      <c r="CJ23" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK23" t="inlineStr">
+        <is>
+          <t>$1,162</t>
+        </is>
+      </c>
+      <c r="CL23" t="n">
+        <v>45</v>
+      </c>
+      <c r="CM23" t="n">
+        <v>117</v>
+      </c>
+      <c r="CN23" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -16231,6 +16658,23 @@
         <v>1</v>
       </c>
       <c r="CI24" t="inlineStr"/>
+      <c r="CJ24" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK24" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL24" t="n">
+        <v>482</v>
+      </c>
+      <c r="CM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN24" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -16504,6 +16948,23 @@
         <v>1</v>
       </c>
       <c r="CI25" t="inlineStr"/>
+      <c r="CJ25" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK25" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL25" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN25" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -16543,7 +17004,7 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>9477</v>
+        <v>7300</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -16556,7 +17017,7 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="O26" t="n">
         <v>10000</v>
@@ -16777,6 +17238,25 @@
         <v>1</v>
       </c>
       <c r="CI26" t="inlineStr"/>
+      <c r="CJ26" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK26" t="inlineStr">
+        <is>
+          <t>$5,310</t>
+        </is>
+      </c>
+      <c r="CL26" t="n">
+        <v>244</v>
+      </c>
+      <c r="CM26" t="n">
+        <v>93</v>
+      </c>
+      <c r="CN26" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -17050,6 +17530,25 @@
         <v>1</v>
       </c>
       <c r="CI27" t="inlineStr"/>
+      <c r="CJ27" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK27" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL27" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN27" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -17323,6 +17822,23 @@
         <v>20</v>
       </c>
       <c r="CI28" t="inlineStr"/>
+      <c r="CJ28" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK28" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL28" t="n">
+        <v>84</v>
+      </c>
+      <c r="CM28" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN28" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -17596,6 +18112,23 @@
         <v>1</v>
       </c>
       <c r="CI29" t="inlineStr"/>
+      <c r="CJ29" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK29" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL29" t="n">
+        <v>63</v>
+      </c>
+      <c r="CM29" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN29" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -17869,6 +18402,23 @@
         <v>1</v>
       </c>
       <c r="CI30" t="inlineStr"/>
+      <c r="CJ30" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK30" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL30" t="n">
+        <v>27</v>
+      </c>
+      <c r="CM30" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN30" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -18142,6 +18692,23 @@
         <v>1</v>
       </c>
       <c r="CI31" t="inlineStr"/>
+      <c r="CJ31" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK31" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL31" t="n">
+        <v>36</v>
+      </c>
+      <c r="CM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN31" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -18415,6 +18982,23 @@
         <v>1</v>
       </c>
       <c r="CI32" t="inlineStr"/>
+      <c r="CJ32" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK32" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL32" t="n">
+        <v>130</v>
+      </c>
+      <c r="CM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN32" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -18688,6 +19272,23 @@
         <v>1</v>
       </c>
       <c r="CI33" t="inlineStr"/>
+      <c r="CJ33" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK33" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL33" t="n">
+        <v>27</v>
+      </c>
+      <c r="CM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN33" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -18961,6 +19562,23 @@
         <v>1</v>
       </c>
       <c r="CI34" t="inlineStr"/>
+      <c r="CJ34" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK34" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL34" t="n">
+        <v>27</v>
+      </c>
+      <c r="CM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN34" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -19234,6 +19852,23 @@
         <v>1</v>
       </c>
       <c r="CI35" t="inlineStr"/>
+      <c r="CJ35" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK35" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL35" t="n">
+        <v>80</v>
+      </c>
+      <c r="CM35" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN35" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -19507,6 +20142,23 @@
         <v>1</v>
       </c>
       <c r="CI36" t="inlineStr"/>
+      <c r="CJ36" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK36" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL36" t="n">
+        <v>244</v>
+      </c>
+      <c r="CM36" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN36" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -19780,6 +20432,23 @@
         <v>1</v>
       </c>
       <c r="CI37" t="inlineStr"/>
+      <c r="CJ37" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK37" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL37" t="n">
+        <v>217</v>
+      </c>
+      <c r="CM37" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN37" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -20053,6 +20722,23 @@
         <v>1</v>
       </c>
       <c r="CI38" t="inlineStr"/>
+      <c r="CJ38" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK38" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL38" t="n">
+        <v>103</v>
+      </c>
+      <c r="CM38" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN38" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -20326,6 +21012,23 @@
         <v>1</v>
       </c>
       <c r="CI39" t="inlineStr"/>
+      <c r="CJ39" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK39" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL39" t="n">
+        <v>151</v>
+      </c>
+      <c r="CM39" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN39" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -20599,6 +21302,23 @@
         <v>1</v>
       </c>
       <c r="CI40" t="inlineStr"/>
+      <c r="CJ40" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK40" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL40" t="n">
+        <v>366</v>
+      </c>
+      <c r="CM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN40" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -20872,6 +21592,23 @@
         <v>1</v>
       </c>
       <c r="CI41" t="inlineStr"/>
+      <c r="CJ41" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK41" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL41" t="n">
+        <v>46</v>
+      </c>
+      <c r="CM41" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN41" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -21145,6 +21882,23 @@
         <v>1</v>
       </c>
       <c r="CI42" t="inlineStr"/>
+      <c r="CJ42" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK42" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL42" t="n">
+        <v>95</v>
+      </c>
+      <c r="CM42" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN42" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -21418,6 +22172,23 @@
         <v>1</v>
       </c>
       <c r="CI43" t="inlineStr"/>
+      <c r="CJ43" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK43" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL43" t="n">
+        <v>272</v>
+      </c>
+      <c r="CM43" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN43" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -21691,6 +22462,23 @@
         <v>1</v>
       </c>
       <c r="CI44" t="inlineStr"/>
+      <c r="CJ44" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK44" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL44" t="n">
+        <v>231</v>
+      </c>
+      <c r="CM44" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN44" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -21964,6 +22752,23 @@
         <v>1</v>
       </c>
       <c r="CI45" t="inlineStr"/>
+      <c r="CJ45" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK45" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL45" t="n">
+        <v>61</v>
+      </c>
+      <c r="CM45" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN45" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -22237,6 +23042,23 @@
         <v>10</v>
       </c>
       <c r="CI46" t="inlineStr"/>
+      <c r="CJ46" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK46" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL46" t="n">
+        <v>45</v>
+      </c>
+      <c r="CM46" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN46" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -22510,6 +23332,25 @@
         <v>20</v>
       </c>
       <c r="CI47" t="inlineStr"/>
+      <c r="CJ47" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK47" t="inlineStr">
+        <is>
+          <t>$380</t>
+        </is>
+      </c>
+      <c r="CL47" t="n">
+        <v>26</v>
+      </c>
+      <c r="CM47" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN47" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -22783,6 +23624,23 @@
         <v>1</v>
       </c>
       <c r="CI48" t="inlineStr"/>
+      <c r="CJ48" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK48" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL48" t="n">
+        <v>267</v>
+      </c>
+      <c r="CM48" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN48" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -23056,6 +23914,23 @@
         <v>1</v>
       </c>
       <c r="CI49" t="inlineStr"/>
+      <c r="CJ49" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK49" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL49" t="n">
+        <v>118</v>
+      </c>
+      <c r="CM49" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN49" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -23329,6 +24204,23 @@
         <v>20</v>
       </c>
       <c r="CI50" t="inlineStr"/>
+      <c r="CJ50" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK50" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL50" t="n">
+        <v>61</v>
+      </c>
+      <c r="CM50" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN50" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -23602,6 +24494,23 @@
         <v>20</v>
       </c>
       <c r="CI51" t="inlineStr"/>
+      <c r="CJ51" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK51" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL51" t="n">
+        <v>211</v>
+      </c>
+      <c r="CM51" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN51" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -23875,6 +24784,23 @@
         <v>1</v>
       </c>
       <c r="CI52" t="inlineStr"/>
+      <c r="CJ52" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK52" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL52" t="n">
+        <v>50</v>
+      </c>
+      <c r="CM52" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN52" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -24148,6 +25074,23 @@
         <v>1</v>
       </c>
       <c r="CI53" t="inlineStr"/>
+      <c r="CJ53" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK53" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL53" t="n">
+        <v>39</v>
+      </c>
+      <c r="CM53" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN53" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -24421,6 +25364,23 @@
         <v>1</v>
       </c>
       <c r="CI54" t="inlineStr"/>
+      <c r="CJ54" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK54" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL54" t="n">
+        <v>424</v>
+      </c>
+      <c r="CM54" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN54" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -24694,6 +25654,23 @@
         <v>1</v>
       </c>
       <c r="CI55" t="inlineStr"/>
+      <c r="CJ55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK55" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL55" t="n">
+        <v>38</v>
+      </c>
+      <c r="CM55" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN55" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -24967,6 +25944,23 @@
         <v>1</v>
       </c>
       <c r="CI56" t="inlineStr"/>
+      <c r="CJ56" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK56" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL56" t="n">
+        <v>226</v>
+      </c>
+      <c r="CM56" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN56" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -25240,6 +26234,23 @@
         <v>1</v>
       </c>
       <c r="CI57" t="inlineStr"/>
+      <c r="CJ57" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK57" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL57" t="n">
+        <v>138</v>
+      </c>
+      <c r="CM57" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN57" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -25513,6 +26524,23 @@
         <v>1</v>
       </c>
       <c r="CI58" t="inlineStr"/>
+      <c r="CJ58" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK58" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL58" t="n">
+        <v>350</v>
+      </c>
+      <c r="CM58" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN58" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -25786,6 +26814,23 @@
         <v>1</v>
       </c>
       <c r="CI59" t="inlineStr"/>
+      <c r="CJ59" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK59" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL59" t="n">
+        <v>562</v>
+      </c>
+      <c r="CM59" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN59" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -26059,6 +27104,23 @@
         <v>18</v>
       </c>
       <c r="CI60" t="inlineStr"/>
+      <c r="CJ60" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK60" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL60" t="n">
+        <v>269</v>
+      </c>
+      <c r="CM60" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN60" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -26332,6 +27394,23 @@
         <v>1</v>
       </c>
       <c r="CI61" t="inlineStr"/>
+      <c r="CJ61" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK61" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL61" t="n">
+        <v>49</v>
+      </c>
+      <c r="CM61" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN61" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -26605,6 +27684,23 @@
         <v>1</v>
       </c>
       <c r="CI62" t="inlineStr"/>
+      <c r="CJ62" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK62" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL62" t="n">
+        <v>30</v>
+      </c>
+      <c r="CM62" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN62" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -26878,6 +27974,23 @@
         <v>14</v>
       </c>
       <c r="CI63" t="inlineStr"/>
+      <c r="CJ63" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK63" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL63" t="n">
+        <v>30</v>
+      </c>
+      <c r="CM63" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN63" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -27151,6 +28264,23 @@
         <v>1</v>
       </c>
       <c r="CI64" t="inlineStr"/>
+      <c r="CJ64" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK64" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL64" t="n">
+        <v>254</v>
+      </c>
+      <c r="CM64" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN64" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -27424,6 +28554,23 @@
         <v>1</v>
       </c>
       <c r="CI65" t="inlineStr"/>
+      <c r="CJ65" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK65" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL65" t="n">
+        <v>30</v>
+      </c>
+      <c r="CM65" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN65" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -27697,6 +28844,23 @@
         <v>1</v>
       </c>
       <c r="CI66" t="inlineStr"/>
+      <c r="CJ66" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK66" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL66" t="n">
+        <v>168</v>
+      </c>
+      <c r="CM66" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN66" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -27970,6 +29134,23 @@
         <v>1</v>
       </c>
       <c r="CI67" t="inlineStr"/>
+      <c r="CJ67" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK67" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL67" t="n">
+        <v>50</v>
+      </c>
+      <c r="CM67" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN67" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -28243,6 +29424,25 @@
         <v>20</v>
       </c>
       <c r="CI68" t="inlineStr"/>
+      <c r="CJ68" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK68" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL68" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM68" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN68" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -28516,6 +29716,25 @@
         <v>1</v>
       </c>
       <c r="CI69" t="inlineStr"/>
+      <c r="CJ69" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK69" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL69" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM69" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN69" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -28789,6 +30008,25 @@
         <v>1</v>
       </c>
       <c r="CI70" t="inlineStr"/>
+      <c r="CJ70" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK70" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL70" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM70" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN70" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -29062,6 +30300,25 @@
         <v>20</v>
       </c>
       <c r="CI71" t="inlineStr"/>
+      <c r="CJ71" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK71" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL71" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM71" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN71" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -29339,6 +30596,25 @@
           <t>Mousehole AFC</t>
         </is>
       </c>
+      <c r="CJ72" t="inlineStr">
+        <is>
+          <t>PartTime</t>
+        </is>
+      </c>
+      <c r="CK72" t="inlineStr">
+        <is>
+          <t>$129</t>
+        </is>
+      </c>
+      <c r="CL72" t="n">
+        <v>19</v>
+      </c>
+      <c r="CM72" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN72" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -29612,6 +30888,25 @@
         <v>1</v>
       </c>
       <c r="CI73" t="inlineStr"/>
+      <c r="CJ73" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK73" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL73" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM73" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN73" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -29885,6 +31180,25 @@
         <v>1</v>
       </c>
       <c r="CI74" t="inlineStr"/>
+      <c r="CJ74" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK74" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL74" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM74" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN74" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -30158,6 +31472,25 @@
         <v>1</v>
       </c>
       <c r="CI75" t="inlineStr"/>
+      <c r="CJ75" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK75" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL75" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM75" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN75" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -30431,6 +31764,25 @@
         <v>1</v>
       </c>
       <c r="CI76" t="inlineStr"/>
+      <c r="CJ76" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK76" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL76" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM76" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN76" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -30704,6 +32056,23 @@
         <v>1</v>
       </c>
       <c r="CI77" t="inlineStr"/>
+      <c r="CJ77" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK77" t="inlineStr">
+        <is>
+          <t>$0</t>
+        </is>
+      </c>
+      <c r="CL77" t="n">
+        <v>27</v>
+      </c>
+      <c r="CM77" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN77" t="n">
+        <v>-1536</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -30981,6 +32350,25 @@
           <t>Tonbridge Angels</t>
         </is>
       </c>
+      <c r="CJ78" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK78" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL78" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM78" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN78" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -31254,6 +32642,25 @@
         <v>1</v>
       </c>
       <c r="CI79" t="inlineStr"/>
+      <c r="CJ79" t="inlineStr">
+        <is>
+          <t>Youth</t>
+        </is>
+      </c>
+      <c r="CK79" t="inlineStr">
+        <is>
+          <t>$29</t>
+        </is>
+      </c>
+      <c r="CL79" t="n">
+        <v>0</v>
+      </c>
+      <c r="CM79" t="n">
+        <v>0</v>
+      </c>
+      <c r="CN79" t="n">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -58317,7 +59724,7 @@
   </sheetPr>
   <dimension ref="A1:AI99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>